<commit_message>
adaptada retenciones para plantilla año 2017 y 2018
</commit_message>
<xml_diff>
--- a/dist/outputs/Retenciones-Estructurado.xlsx
+++ b/dist/outputs/Retenciones-Estructurado.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Concepto</t>
   </si>
@@ -49,7 +49,7 @@
     <t>Servicios (Base sujeta a retención para pagos o abonos en cuenta)</t>
   </si>
   <si>
-    <t>Rendimientos financieros e intereses (Base sujeta a retención para pagos o abonos en cuenta)</t>
+    <t>Rendimientos financieros (Base sujeta a retención para pagos o abonos en cuenta)</t>
   </si>
   <si>
     <t>Arrendamientos (Muebles e inmuebles) (Base sujeta a retención para pagos o abonos en cuenta)</t>
@@ -79,7 +79,7 @@
     <t>Otros pagos sujetos a retención (Base sujeta a retención para pagos o abonos en cuenta)</t>
   </si>
   <si>
-    <t>Autorretenciones - Contribuyentes exonerados de aportes (art. 114-1 E.T.) (Base sujeta a retención para pagos o abonos en cuenta)</t>
+    <t>Autorretenciones - Decreto 2201 de 2016  (Base sujeta a retención para pagos o abonos en cuenta)</t>
   </si>
   <si>
     <t>Autorretenciones - Ventas (Base sujeta a retención para pagos o abonos en cuenta)</t>
@@ -97,9 +97,6 @@
     <t>Autorretenciones - Rendimientos financieros (Base sujeta a retención para pagos o abonos en cuenta)</t>
   </si>
   <si>
-    <t>Autorretenciones - Pagos mensuales provisionales de carácter voluntario (hidrocarburos y demás productos mineros) (Base sujeta a retención para pagos o abonos en cuenta)</t>
-  </si>
-  <si>
     <t>Autorretenciones - Otros conceptos (Base sujeta a retención para pagos o abonos en cuenta)</t>
   </si>
   <si>
@@ -124,7 +121,7 @@
     <t>Servicios(Retenciones a título de renta)</t>
   </si>
   <si>
-    <t>Rendimientos financieros e intereses(Retenciones a título de renta)</t>
+    <t>Rendimientos financieros (Retenciones a título de renta)</t>
   </si>
   <si>
     <t>Arrendamientos (Muebles e inmuebles)(Retenciones a título de renta)</t>
@@ -154,7 +151,7 @@
     <t>Otros pagos sujetos a retención(Retenciones a título de renta)</t>
   </si>
   <si>
-    <t>Autorretenciones - Contribuyentes exonerados de aportes (art. 114-1 E.T.)(Retenciones a título de renta)</t>
+    <t>Autorretenciones - Decreto 2201 de 2016 (Retenciones a título de renta)</t>
   </si>
   <si>
     <t>Autorretenciones - Ventas(Retenciones a título de renta)</t>
@@ -172,9 +169,6 @@
     <t>Autorretenciones - Rendimientos financieros(Retenciones a título de renta)</t>
   </si>
   <si>
-    <t>Autorretenciones - Pagos mensuales provisionales de carácter voluntario (hidrocarburos y demás productos mineros)(Retenciones a título de renta)</t>
-  </si>
-  <si>
     <t>Autorretenciones - Otros conceptos(Retenciones a título de renta)</t>
   </si>
   <si>
@@ -203,9 +197,6 @@
   </si>
   <si>
     <t>Retenciones impuesto timbre nacional</t>
-  </si>
-  <si>
-    <t>Retenciones impuesto nacional al consumo</t>
   </si>
   <si>
     <t>Total retenciones</t>
@@ -273,7 +264,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -308,10 +299,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
@@ -328,7 +319,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>6</v>
@@ -345,7 +336,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>6</v>
@@ -362,7 +353,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>6</v>
@@ -379,7 +370,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>6</v>
@@ -393,10 +384,10 @@
         <v>31</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>0</v>
+        <v>59000</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>6</v>
@@ -413,7 +404,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>6</v>
@@ -427,10 +418,10 @@
         <v>33</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>3706000</v>
+        <v>3327000</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>6</v>
@@ -447,7 +438,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>6</v>
@@ -464,7 +455,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>6</v>
@@ -481,7 +472,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>6</v>
@@ -498,7 +489,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>6</v>
@@ -515,7 +506,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>6</v>
@@ -532,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>6</v>
@@ -549,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>6</v>
@@ -563,10 +554,10 @@
         <v>41</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>0</v>
+        <v>11864000</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>6</v>
@@ -580,10 +571,10 @@
         <v>42</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>14260000</v>
+        <v>19677000</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>6</v>
@@ -600,7 +591,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>6</v>
@@ -617,7 +608,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>6</v>
@@ -634,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>6</v>
@@ -651,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>6</v>
@@ -668,7 +659,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>6</v>
@@ -685,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>6</v>
@@ -702,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>6</v>
@@ -719,7 +710,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>6</v>
@@ -736,7 +727,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>6</v>
@@ -753,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>6</v>
@@ -770,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>6</v>
@@ -787,7 +778,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>6</v>
@@ -801,10 +792,10 @@
         <v>55</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>6</v>
@@ -821,7 +812,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>6</v>
@@ -835,10 +826,10 @@
         <v>57</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>0</v>
+        <v>98000</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>6</v>
@@ -852,10 +843,10 @@
         <v>58</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>109000</v>
+        <v>0</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>6</v>
@@ -872,7 +863,7 @@
         <v>0</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>6</v>
@@ -889,7 +880,7 @@
         <v>0</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>6</v>
@@ -906,7 +897,7 @@
         <v>0</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>6</v>
@@ -923,7 +914,7 @@
         <v>0</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>6</v>
@@ -940,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>6</v>
@@ -957,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>6</v>
@@ -971,10 +962,10 @@
         <v>65</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>0</v>
+        <v>415000</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>6</v>
@@ -988,10 +979,10 @@
         <v>66</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>0</v>
+        <v>157000</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>6</v>
@@ -1005,10 +996,10 @@
         <v>67</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>114000</v>
+        <v>0</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>6</v>
@@ -1025,7 +1016,7 @@
         <v>0</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>6</v>
@@ -1042,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>6</v>
@@ -1059,7 +1050,7 @@
         <v>0</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>6</v>
@@ -1076,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>6</v>
@@ -1093,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>6</v>
@@ -1110,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>6</v>
@@ -1127,7 +1118,7 @@
         <v>0</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>6</v>
@@ -1144,7 +1135,7 @@
         <v>0</v>
       </c>
       <c r="D51" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>6</v>
@@ -1158,10 +1149,10 @@
         <v>76</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>0</v>
+        <v>671000</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>6</v>
@@ -1178,7 +1169,7 @@
         <v>0</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>6</v>
@@ -1192,10 +1183,10 @@
         <v>78</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>223000</v>
+        <v>0</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>6</v>
@@ -1212,7 +1203,7 @@
         <v>0</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>6</v>
@@ -1229,7 +1220,7 @@
         <v>0</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>6</v>
@@ -1246,7 +1237,7 @@
         <v>0</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>6</v>
@@ -1260,10 +1251,10 @@
         <v>82</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>0</v>
+        <v>671000</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>6</v>
@@ -1280,7 +1271,7 @@
         <v>0</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>6</v>
@@ -1294,10 +1285,10 @@
         <v>84</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>0</v>
+        <v>671000</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>6</v>
@@ -1308,66 +1299,15 @@
         <v>65</v>
       </c>
       <c r="B61" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="C61" s="1" t="n">
-        <v>223000</v>
+        <v>91</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" customHeight="1">
-      <c r="A62" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B62" s="1" t="n">
-        <v>86</v>
-      </c>
-      <c r="C62" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="D62" s="1" t="n">
-        <v>2019</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" customHeight="1">
-      <c r="A63" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B63" s="1" t="n">
-        <v>87</v>
-      </c>
-      <c r="C63" s="1" t="n">
-        <v>223000</v>
-      </c>
-      <c r="D63" s="1" t="n">
-        <v>2019</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" customHeight="1">
-      <c r="A64" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B64" s="1" t="n">
-        <v>91</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D64" s="1" t="n">
-        <v>2019</v>
-      </c>
-      <c r="E64" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>